<commit_message>
Replaced 2.5mm MDF with 2mm
</commit_message>
<xml_diff>
--- a/physical-build-resources/DE-Arm-BoM.xlsx
+++ b/physical-build-resources/DE-Arm-BoM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{E0A7FF59-95F5-0941-8588-437375E973B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC815938-2802-7A40-B23C-876F30D37FBE}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{E0A7FF59-95F5-0941-8588-437375E973B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{980BBEB6-7A97-4140-AC36-94E5BA7FDACA}"/>
   <bookViews>
     <workbookView xWindow="-24180" yWindow="5040" windowWidth="14160" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,6 @@
     <t>DE Arm 25 4mm Parts</t>
   </si>
   <si>
-    <t>DE Arm 25 2.5mm Parts</t>
-  </si>
-  <si>
     <t>SG90 - Micro Servo 9g</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Stick-on Feet</t>
+  </si>
+  <si>
+    <t>DE Arm 25 2mm Parts</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,7 +471,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -493,23 +493,23 @@
         <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>13</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
@@ -553,24 +553,24 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>